<commit_message>
Restante dos métodos. ERRO no bloquear/desbloquear Vertice ou Criar Aresta?
</commit_message>
<xml_diff>
--- a/resources/args.xlsx
+++ b/resources/args.xlsx
@@ -1,16 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steff\OneDrive\Documentos\UFU\6º Período\Sistemas Distribuídos\bdgrafo\ThriftGrafoSD\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="args" sheetId="4" r:id="rId1"/>
-    <sheet name="Plan1" sheetId="1" r:id="rId2"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId3"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621" calcMode="manual"/>
 </workbook>
@@ -208,7 +210,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -415,7 +417,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -433,7 +435,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -471,7 +473,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -506,23 +508,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -558,26 +543,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -750,36 +718,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.31640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.22265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.4140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.02734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.43359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.22265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.43359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.22265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.43359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.43359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.4140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.02734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.14453125" style="1"/>
+    <col min="1" max="1" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
@@ -1339,40 +1307,4 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Remoção de opções do Cliente Impressão nos Command e Querys para mostrar a replicação ocorrendo
</commit_message>
<xml_diff>
--- a/resources/args.xlsx
+++ b/resources/args.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="64">
   <si>
     <t>Parâmetros referentes ao servidor que o cliente irá se conectar (somente portas Thrift interessam), tamanho 2 x N</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>localhost 9094 9095 false localhost 9092 9093 localhost 9090 9091 5 localhost 7070 localhost 7072 localhost 7074 localhost 8080 localhost 8082 localhost 8084</t>
+  </si>
+  <si>
+    <t>java -jar Client.jar</t>
+  </si>
+  <si>
+    <t>java-jar Server.jar</t>
   </si>
 </sst>
 </file>
@@ -721,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1220,6 +1226,9 @@
         <v>49</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1228,6 +1237,9 @@
         <v>40</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1236,6 +1248,9 @@
         <v>41</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1244,6 +1259,9 @@
         <v>42</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1252,46 +1270,64 @@
         <v>43</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>